<commit_message>
Added script and files related to growth and pca analysis.
</commit_message>
<xml_diff>
--- a/BiologAnalysis/output/AUC/rsol_time_WT_AUCsPM 1-.xlsx
+++ b/BiologAnalysis/output/AUC/rsol_time_WT_AUCsPM 1-.xlsx
@@ -17,6 +17,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
   <si>
+    <t>CFBP2957 replicate 1</t>
+  </si>
+  <si>
+    <t>CFBP2957 replicate 2</t>
+  </si>
+  <si>
+    <t>CFBP2957 replicate 3</t>
+  </si>
+  <si>
     <t>BA7 replicate 1</t>
   </si>
   <si>
@@ -33,15 +42,6 @@
   </si>
   <si>
     <t>BDBR229 replicate 3</t>
-  </si>
-  <si>
-    <t>CFBP2957 replicate 1</t>
-  </si>
-  <si>
-    <t>CFBP2957 replicate 2</t>
-  </si>
-  <si>
-    <t>CFBP2957 replicate 3</t>
   </si>
   <si>
     <t>GMI1000 replicate 1</t>
@@ -974,31 +974,31 @@
         <v>34</v>
       </c>
       <c r="B3" t="n">
+        <v>92.75</v>
+      </c>
+      <c r="C3" t="n">
+        <v>610.75</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22.125</v>
+      </c>
+      <c r="E3" t="n">
         <v>113.5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="F3" t="n">
         <v>291.25</v>
       </c>
-      <c r="D3" t="n">
+      <c r="G3" t="n">
         <v>43.375</v>
       </c>
-      <c r="E3" t="n">
+      <c r="H3" t="n">
         <v>5.5</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>187</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>20.625</v>
-      </c>
-      <c r="H3" t="n">
-        <v>92.75</v>
-      </c>
-      <c r="I3" t="n">
-        <v>610.75</v>
-      </c>
-      <c r="J3" t="n">
-        <v>22.125</v>
       </c>
       <c r="K3" t="n">
         <v>2.75</v>
@@ -1081,31 +1081,31 @@
         <v>35</v>
       </c>
       <c r="B4" t="n">
+        <v>2828.625</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2737.875</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1804.25</v>
+      </c>
+      <c r="E4" t="n">
         <v>2912.25</v>
       </c>
-      <c r="C4" t="n">
+      <c r="F4" t="n">
         <v>2886.5</v>
       </c>
-      <c r="D4" t="n">
+      <c r="G4" t="n">
         <v>2850.5</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
       <c r="H4" t="n">
-        <v>2828.625</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>2737.875</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>1804.25</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>845.125</v>
@@ -1188,31 +1188,31 @@
         <v>36</v>
       </c>
       <c r="B5" t="n">
+        <v>9242.875</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9227</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8405.25</v>
+      </c>
+      <c r="E5" t="n">
         <v>8889.75</v>
       </c>
-      <c r="C5" t="n">
+      <c r="F5" t="n">
         <v>8536.625</v>
       </c>
-      <c r="D5" t="n">
+      <c r="G5" t="n">
         <v>9727.5</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
       <c r="H5" t="n">
-        <v>9242.875</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>9227</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>8405.25</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>7176.625</v>
@@ -1295,31 +1295,31 @@
         <v>37</v>
       </c>
       <c r="B6" t="n">
+        <v>3563.875</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3177.125</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2062.625</v>
+      </c>
+      <c r="E6" t="n">
         <v>7627.375</v>
       </c>
-      <c r="C6" t="n">
+      <c r="F6" t="n">
         <v>8015.875</v>
       </c>
-      <c r="D6" t="n">
+      <c r="G6" t="n">
         <v>6767.25</v>
       </c>
-      <c r="E6" t="n">
+      <c r="H6" t="n">
         <v>5011.25</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
         <v>4191.75</v>
       </c>
-      <c r="G6" t="n">
+      <c r="J6" t="n">
         <v>5895.5</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3563.875</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3177.125</v>
-      </c>
-      <c r="J6" t="n">
-        <v>2062.625</v>
       </c>
       <c r="K6" t="n">
         <v>6657.375</v>
@@ -1402,31 +1402,31 @@
         <v>38</v>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>7.5</v>
       </c>
-      <c r="C7" t="n">
+      <c r="F7" t="n">
         <v>1.5</v>
       </c>
-      <c r="D7" t="n">
+      <c r="G7" t="n">
         <v>5.75</v>
       </c>
-      <c r="E7" t="n">
+      <c r="H7" t="n">
         <v>3.25</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
         <v>2</v>
       </c>
-      <c r="G7" t="n">
+      <c r="J7" t="n">
         <v>3.75</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>5152.25</v>
@@ -1509,31 +1509,31 @@
         <v>39</v>
       </c>
       <c r="B8" t="n">
+        <v>9035.75</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8403.25</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7965.875</v>
+      </c>
+      <c r="E8" t="n">
         <v>9458</v>
       </c>
-      <c r="C8" t="n">
+      <c r="F8" t="n">
         <v>11146.625</v>
       </c>
-      <c r="D8" t="n">
+      <c r="G8" t="n">
         <v>12909.625</v>
       </c>
-      <c r="E8" t="n">
+      <c r="H8" t="n">
         <v>5245.625</v>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
         <v>4235.75</v>
       </c>
-      <c r="G8" t="n">
+      <c r="J8" t="n">
         <v>7083.75</v>
-      </c>
-      <c r="H8" t="n">
-        <v>9035.75</v>
-      </c>
-      <c r="I8" t="n">
-        <v>8403.25</v>
-      </c>
-      <c r="J8" t="n">
-        <v>7965.875</v>
       </c>
       <c r="K8" t="n">
         <v>11748.375</v>
@@ -1616,31 +1616,31 @@
         <v>40</v>
       </c>
       <c r="B9" t="n">
+        <v>337.75</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500.25</v>
+      </c>
+      <c r="D9" t="n">
+        <v>401.875</v>
+      </c>
+      <c r="E9" t="n">
         <v>8179</v>
       </c>
-      <c r="C9" t="n">
+      <c r="F9" t="n">
         <v>7250.875</v>
       </c>
-      <c r="D9" t="n">
+      <c r="G9" t="n">
         <v>7799.125</v>
       </c>
-      <c r="E9" t="n">
+      <c r="H9" t="n">
         <v>267</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
         <v>286.5</v>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
         <v>630</v>
-      </c>
-      <c r="H9" t="n">
-        <v>337.75</v>
-      </c>
-      <c r="I9" t="n">
-        <v>500.25</v>
-      </c>
-      <c r="J9" t="n">
-        <v>401.875</v>
       </c>
       <c r="K9" t="n">
         <v>0.5</v>
@@ -1723,31 +1723,31 @@
         <v>41</v>
       </c>
       <c r="B10" t="n">
+        <v>19</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
         <v>3784.75</v>
       </c>
-      <c r="C10" t="n">
+      <c r="F10" t="n">
         <v>3129.25</v>
       </c>
-      <c r="D10" t="n">
+      <c r="G10" t="n">
         <v>3477</v>
       </c>
-      <c r="E10" t="n">
+      <c r="H10" t="n">
         <v>7.5</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
         <v>0.25</v>
       </c>
-      <c r="G10" t="n">
+      <c r="J10" t="n">
         <v>32.625</v>
-      </c>
-      <c r="H10" t="n">
-        <v>19</v>
-      </c>
-      <c r="I10" t="n">
-        <v>8.75</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -1830,31 +1830,31 @@
         <v>42</v>
       </c>
       <c r="B11" t="n">
+        <v>9343.125</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9452.75</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8957.375</v>
+      </c>
+      <c r="E11" t="n">
         <v>9190</v>
       </c>
-      <c r="C11" t="n">
+      <c r="F11" t="n">
         <v>9969.625</v>
       </c>
-      <c r="D11" t="n">
+      <c r="G11" t="n">
         <v>9533.375</v>
       </c>
-      <c r="E11" t="n">
+      <c r="H11" t="n">
         <v>0.5</v>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
         <v>0.5</v>
       </c>
-      <c r="G11" t="n">
+      <c r="J11" t="n">
         <v>3.5</v>
-      </c>
-      <c r="H11" t="n">
-        <v>9343.125</v>
-      </c>
-      <c r="I11" t="n">
-        <v>9452.75</v>
-      </c>
-      <c r="J11" t="n">
-        <v>8957.375</v>
       </c>
       <c r="K11" t="n">
         <v>10943.375</v>
@@ -1937,31 +1937,31 @@
         <v>43</v>
       </c>
       <c r="B12" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="C12" t="n">
+        <v>194</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
         <v>207.875</v>
       </c>
-      <c r="C12" t="n">
+      <c r="F12" t="n">
         <v>8.125</v>
       </c>
-      <c r="D12" t="n">
+      <c r="G12" t="n">
         <v>231.25</v>
       </c>
-      <c r="E12" t="n">
+      <c r="H12" t="n">
         <v>118.875</v>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
         <v>19.75</v>
       </c>
-      <c r="G12" t="n">
+      <c r="J12" t="n">
         <v>155.625</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="I12" t="n">
-        <v>194</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1</v>
       </c>
       <c r="K12" t="n">
         <v>4.375</v>
@@ -2044,31 +2044,31 @@
         <v>44</v>
       </c>
       <c r="B13" t="n">
+        <v>536.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>693.375</v>
+      </c>
+      <c r="D13" t="n">
+        <v>308.375</v>
+      </c>
+      <c r="E13" t="n">
         <v>1047.75</v>
       </c>
-      <c r="C13" t="n">
+      <c r="F13" t="n">
         <v>1986.375</v>
       </c>
-      <c r="D13" t="n">
+      <c r="G13" t="n">
         <v>831</v>
       </c>
-      <c r="E13" t="n">
+      <c r="H13" t="n">
         <v>343.5</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
         <v>415.125</v>
       </c>
-      <c r="G13" t="n">
+      <c r="J13" t="n">
         <v>347.5</v>
-      </c>
-      <c r="H13" t="n">
-        <v>536.5</v>
-      </c>
-      <c r="I13" t="n">
-        <v>693.375</v>
-      </c>
-      <c r="J13" t="n">
-        <v>308.375</v>
       </c>
       <c r="K13" t="n">
         <v>10429.25</v>
@@ -2151,31 +2151,31 @@
         <v>45</v>
       </c>
       <c r="B14" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
         <v>514.625</v>
       </c>
-      <c r="C14" t="n">
+      <c r="F14" t="n">
         <v>178.375</v>
       </c>
-      <c r="D14" t="n">
+      <c r="G14" t="n">
         <v>527</v>
       </c>
-      <c r="E14" t="n">
+      <c r="H14" t="n">
         <v>25</v>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
         <v>3.25</v>
       </c>
-      <c r="G14" t="n">
+      <c r="J14" t="n">
         <v>54.625</v>
-      </c>
-      <c r="H14" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -2258,16 +2258,16 @@
         <v>46</v>
       </c>
       <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
         <v>1.25</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2365,31 +2365,31 @@
         <v>47</v>
       </c>
       <c r="B16" t="n">
+        <v>1483.125</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1117.5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>896</v>
+      </c>
+      <c r="E16" t="n">
         <v>3389.5</v>
       </c>
-      <c r="C16" t="n">
+      <c r="F16" t="n">
         <v>3074.375</v>
       </c>
-      <c r="D16" t="n">
+      <c r="G16" t="n">
         <v>2245</v>
       </c>
-      <c r="E16" t="n">
+      <c r="H16" t="n">
         <v>8.25</v>
       </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="n">
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
         <v>41.625</v>
-      </c>
-      <c r="H16" t="n">
-        <v>1483.125</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1117.5</v>
-      </c>
-      <c r="J16" t="n">
-        <v>896</v>
       </c>
       <c r="K16" t="n">
         <v>4195.125</v>
@@ -2472,25 +2472,25 @@
         <v>48</v>
       </c>
       <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
         <v>24.25</v>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
         <v>3.75</v>
       </c>
-      <c r="E17" t="n">
+      <c r="H17" t="n">
         <v>0.25</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -2579,31 +2579,31 @@
         <v>49</v>
       </c>
       <c r="B18" t="n">
+        <v>8359.75</v>
+      </c>
+      <c r="C18" t="n">
+        <v>7628.125</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7212.25</v>
+      </c>
+      <c r="E18" t="n">
         <v>9345.75</v>
       </c>
-      <c r="C18" t="n">
+      <c r="F18" t="n">
         <v>8210.125</v>
       </c>
-      <c r="D18" t="n">
+      <c r="G18" t="n">
         <v>8341.125</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
       <c r="H18" t="n">
-        <v>8359.75</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>7628.125</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>7212.25</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>13269.75</v>
@@ -2686,31 +2686,31 @@
         <v>50</v>
       </c>
       <c r="B19" t="n">
+        <v>2166</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2104.375</v>
+      </c>
+      <c r="D19" t="n">
+        <v>945.625</v>
+      </c>
+      <c r="E19" t="n">
         <v>4991.375</v>
       </c>
-      <c r="C19" t="n">
+      <c r="F19" t="n">
         <v>4595.125</v>
       </c>
-      <c r="D19" t="n">
+      <c r="G19" t="n">
         <v>4031</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
-      </c>
       <c r="H19" t="n">
-        <v>2166</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>2104.375</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>945.625</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
         <v>3026.5</v>
@@ -2900,31 +2900,31 @@
         <v>52</v>
       </c>
       <c r="B21" t="n">
+        <v>14.25</v>
+      </c>
+      <c r="C21" t="n">
+        <v>14.25</v>
+      </c>
+      <c r="D21" t="n">
+        <v>46.375</v>
+      </c>
+      <c r="E21" t="n">
         <v>343.125</v>
       </c>
-      <c r="C21" t="n">
+      <c r="F21" t="n">
         <v>5.375</v>
       </c>
-      <c r="D21" t="n">
+      <c r="G21" t="n">
         <v>172.5</v>
       </c>
-      <c r="E21" t="n">
+      <c r="H21" t="n">
         <v>29.875</v>
       </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
         <v>50.25</v>
-      </c>
-      <c r="H21" t="n">
-        <v>14.25</v>
-      </c>
-      <c r="I21" t="n">
-        <v>14.25</v>
-      </c>
-      <c r="J21" t="n">
-        <v>46.375</v>
       </c>
       <c r="K21" t="n">
         <v>1.5</v>
@@ -3007,31 +3007,31 @@
         <v>53</v>
       </c>
       <c r="B22" t="n">
+        <v>524.25</v>
+      </c>
+      <c r="C22" t="n">
+        <v>392.375</v>
+      </c>
+      <c r="D22" t="n">
+        <v>348.125</v>
+      </c>
+      <c r="E22" t="n">
         <v>122.875</v>
       </c>
-      <c r="C22" t="n">
+      <c r="F22" t="n">
         <v>65.5</v>
       </c>
-      <c r="D22" t="n">
+      <c r="G22" t="n">
         <v>60.375</v>
       </c>
-      <c r="E22" t="n">
+      <c r="H22" t="n">
         <v>1</v>
       </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
         <v>30.75</v>
-      </c>
-      <c r="H22" t="n">
-        <v>524.25</v>
-      </c>
-      <c r="I22" t="n">
-        <v>392.375</v>
-      </c>
-      <c r="J22" t="n">
-        <v>348.125</v>
       </c>
       <c r="K22" t="n">
         <v>4541.75</v>
@@ -3114,31 +3114,31 @@
         <v>54</v>
       </c>
       <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
         <v>44.25</v>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
         <v>85.25</v>
       </c>
-      <c r="E23" t="n">
+      <c r="H23" t="n">
         <v>2</v>
       </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
         <v>8.625</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
@@ -3221,31 +3221,31 @@
         <v>55</v>
       </c>
       <c r="B24" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
         <v>75.625</v>
       </c>
-      <c r="C24" t="n">
+      <c r="F24" t="n">
         <v>10.125</v>
       </c>
-      <c r="D24" t="n">
+      <c r="G24" t="n">
         <v>133.75</v>
       </c>
-      <c r="E24" t="n">
+      <c r="H24" t="n">
         <v>8</v>
       </c>
-      <c r="F24" t="n">
+      <c r="I24" t="n">
         <v>1</v>
       </c>
-      <c r="G24" t="n">
+      <c r="J24" t="n">
         <v>16</v>
-      </c>
-      <c r="H24" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>0</v>
       </c>
       <c r="K24" t="n">
         <v>3380.25</v>
@@ -3328,31 +3328,31 @@
         <v>56</v>
       </c>
       <c r="B25" t="n">
+        <v>11540.25</v>
+      </c>
+      <c r="C25" t="n">
+        <v>11028.25</v>
+      </c>
+      <c r="D25" t="n">
+        <v>10507.25</v>
+      </c>
+      <c r="E25" t="n">
         <v>13380</v>
       </c>
-      <c r="C25" t="n">
+      <c r="F25" t="n">
         <v>12232.875</v>
       </c>
-      <c r="D25" t="n">
+      <c r="G25" t="n">
         <v>12781.25</v>
       </c>
-      <c r="E25" t="n">
+      <c r="H25" t="n">
         <v>7290.75</v>
       </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
         <v>6622.625</v>
       </c>
-      <c r="G25" t="n">
+      <c r="J25" t="n">
         <v>9468.5</v>
-      </c>
-      <c r="H25" t="n">
-        <v>11540.25</v>
-      </c>
-      <c r="I25" t="n">
-        <v>11028.25</v>
-      </c>
-      <c r="J25" t="n">
-        <v>10507.25</v>
       </c>
       <c r="K25" t="n">
         <v>12777.75</v>
@@ -3435,31 +3435,31 @@
         <v>57</v>
       </c>
       <c r="B26" t="n">
+        <v>21.75</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
         <v>277.375</v>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
         <v>286</v>
       </c>
-      <c r="E26" t="n">
+      <c r="H26" t="n">
         <v>215.625</v>
       </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
         <v>228.125</v>
-      </c>
-      <c r="H26" t="n">
-        <v>21.75</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0</v>
       </c>
       <c r="K26" t="n">
         <v>0.25</v>
@@ -3649,31 +3649,31 @@
         <v>59</v>
       </c>
       <c r="B28" t="n">
+        <v>7179.625</v>
+      </c>
+      <c r="C28" t="n">
+        <v>6388.625</v>
+      </c>
+      <c r="D28" t="n">
+        <v>5775.25</v>
+      </c>
+      <c r="E28" t="n">
         <v>10590</v>
       </c>
-      <c r="C28" t="n">
+      <c r="F28" t="n">
         <v>9863.125</v>
       </c>
-      <c r="D28" t="n">
+      <c r="G28" t="n">
         <v>10601.25</v>
       </c>
-      <c r="E28" t="n">
+      <c r="H28" t="n">
         <v>3018.25</v>
       </c>
-      <c r="F28" t="n">
+      <c r="I28" t="n">
         <v>1445.875</v>
       </c>
-      <c r="G28" t="n">
+      <c r="J28" t="n">
         <v>3601.125</v>
-      </c>
-      <c r="H28" t="n">
-        <v>7179.625</v>
-      </c>
-      <c r="I28" t="n">
-        <v>6388.625</v>
-      </c>
-      <c r="J28" t="n">
-        <v>5775.25</v>
       </c>
       <c r="K28" t="n">
         <v>10239.375</v>
@@ -3756,31 +3756,31 @@
         <v>60</v>
       </c>
       <c r="B29" t="n">
+        <v>402.625</v>
+      </c>
+      <c r="C29" t="n">
+        <v>60.375</v>
+      </c>
+      <c r="D29" t="n">
+        <v>18</v>
+      </c>
+      <c r="E29" t="n">
         <v>242.25</v>
       </c>
-      <c r="C29" t="n">
+      <c r="F29" t="n">
         <v>25.875</v>
       </c>
-      <c r="D29" t="n">
+      <c r="G29" t="n">
         <v>239</v>
       </c>
-      <c r="E29" t="n">
+      <c r="H29" t="n">
         <v>297.375</v>
       </c>
-      <c r="F29" t="n">
+      <c r="I29" t="n">
         <v>11</v>
       </c>
-      <c r="G29" t="n">
+      <c r="J29" t="n">
         <v>325.125</v>
-      </c>
-      <c r="H29" t="n">
-        <v>402.625</v>
-      </c>
-      <c r="I29" t="n">
-        <v>60.375</v>
-      </c>
-      <c r="J29" t="n">
-        <v>18</v>
       </c>
       <c r="K29" t="n">
         <v>9.75</v>
@@ -3863,31 +3863,31 @@
         <v>61</v>
       </c>
       <c r="B30" t="n">
+        <v>5051.375</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4729.25</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3715.625</v>
+      </c>
+      <c r="E30" t="n">
         <v>5379.5</v>
       </c>
-      <c r="C30" t="n">
+      <c r="F30" t="n">
         <v>4785.625</v>
       </c>
-      <c r="D30" t="n">
+      <c r="G30" t="n">
         <v>4938</v>
       </c>
-      <c r="E30" t="n">
+      <c r="H30" t="n">
         <v>782.625</v>
       </c>
-      <c r="F30" t="n">
+      <c r="I30" t="n">
         <v>332.75</v>
       </c>
-      <c r="G30" t="n">
+      <c r="J30" t="n">
         <v>1431.25</v>
-      </c>
-      <c r="H30" t="n">
-        <v>5051.375</v>
-      </c>
-      <c r="I30" t="n">
-        <v>4729.25</v>
-      </c>
-      <c r="J30" t="n">
-        <v>3715.625</v>
       </c>
       <c r="K30" t="n">
         <v>6859.25</v>
@@ -3970,22 +3970,22 @@
         <v>62</v>
       </c>
       <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
         <v>2.75</v>
       </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="n">
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
         <v>1.25</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -4077,31 +4077,31 @@
         <v>63</v>
       </c>
       <c r="B32" t="n">
+        <v>108.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="D32" t="n">
+        <v>9</v>
+      </c>
+      <c r="E32" t="n">
         <v>291.125</v>
       </c>
-      <c r="C32" t="n">
+      <c r="F32" t="n">
         <v>56</v>
       </c>
-      <c r="D32" t="n">
+      <c r="G32" t="n">
         <v>276.875</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0</v>
-      </c>
       <c r="H32" t="n">
-        <v>108.5</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>23.5</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K32" t="n">
         <v>559</v>
@@ -4184,31 +4184,31 @@
         <v>64</v>
       </c>
       <c r="B33" t="n">
+        <v>2975.625</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2488.5</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2577.625</v>
+      </c>
+      <c r="E33" t="n">
         <v>4752.5</v>
       </c>
-      <c r="C33" t="n">
+      <c r="F33" t="n">
         <v>3301.25</v>
       </c>
-      <c r="D33" t="n">
+      <c r="G33" t="n">
         <v>3996.875</v>
       </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
       <c r="H33" t="n">
-        <v>2975.625</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>2488.5</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>2577.625</v>
+        <v>0</v>
       </c>
       <c r="K33" t="n">
         <v>3233.375</v>
@@ -4291,31 +4291,31 @@
         <v>65</v>
       </c>
       <c r="B34" t="n">
+        <v>9346.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8527.75</v>
+      </c>
+      <c r="D34" t="n">
+        <v>8635.5</v>
+      </c>
+      <c r="E34" t="n">
         <v>9894.125</v>
       </c>
-      <c r="C34" t="n">
+      <c r="F34" t="n">
         <v>8830.25</v>
       </c>
-      <c r="D34" t="n">
+      <c r="G34" t="n">
         <v>9775.5</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
         <v>0.5</v>
-      </c>
-      <c r="H34" t="n">
-        <v>9346.5</v>
-      </c>
-      <c r="I34" t="n">
-        <v>8527.75</v>
-      </c>
-      <c r="J34" t="n">
-        <v>8635.5</v>
       </c>
       <c r="K34" t="n">
         <v>11422.875</v>
@@ -4398,31 +4398,31 @@
         <v>66</v>
       </c>
       <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
         <v>2.5</v>
       </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
         <v>16</v>
       </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
         <v>0.25</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>0</v>
       </c>
       <c r="K35" t="n">
         <v>0</v>
@@ -4505,31 +4505,31 @@
         <v>67</v>
       </c>
       <c r="B36" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
         <v>39.5</v>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
         <v>49.375</v>
       </c>
-      <c r="E36" t="n">
+      <c r="H36" t="n">
         <v>11.5</v>
       </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
         <v>27.75</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0</v>
       </c>
       <c r="K36" t="n">
         <v>0</v>
@@ -4612,31 +4612,31 @@
         <v>68</v>
       </c>
       <c r="B37" t="n">
+        <v>45</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E37" t="n">
         <v>632.875</v>
       </c>
-      <c r="C37" t="n">
+      <c r="F37" t="n">
         <v>2</v>
       </c>
-      <c r="D37" t="n">
+      <c r="G37" t="n">
         <v>732.375</v>
       </c>
-      <c r="E37" t="n">
+      <c r="H37" t="n">
         <v>765.25</v>
       </c>
-      <c r="F37" t="n">
+      <c r="I37" t="n">
         <v>0.25</v>
       </c>
-      <c r="G37" t="n">
+      <c r="J37" t="n">
         <v>657.25</v>
-      </c>
-      <c r="H37" t="n">
-        <v>45</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J37" t="n">
-        <v>3.5</v>
       </c>
       <c r="K37" t="n">
         <v>32.5</v>
@@ -4719,31 +4719,31 @@
         <v>69</v>
       </c>
       <c r="B38" t="n">
+        <v>9910.875</v>
+      </c>
+      <c r="C38" t="n">
+        <v>9281.875</v>
+      </c>
+      <c r="D38" t="n">
+        <v>8571.5</v>
+      </c>
+      <c r="E38" t="n">
         <v>13330.25</v>
       </c>
-      <c r="C38" t="n">
+      <c r="F38" t="n">
         <v>12309.625</v>
       </c>
-      <c r="D38" t="n">
+      <c r="G38" t="n">
         <v>13263.5</v>
       </c>
-      <c r="E38" t="n">
+      <c r="H38" t="n">
         <v>5530.5</v>
       </c>
-      <c r="F38" t="n">
+      <c r="I38" t="n">
         <v>4700.625</v>
       </c>
-      <c r="G38" t="n">
+      <c r="J38" t="n">
         <v>7214.25</v>
-      </c>
-      <c r="H38" t="n">
-        <v>9910.875</v>
-      </c>
-      <c r="I38" t="n">
-        <v>9281.875</v>
-      </c>
-      <c r="J38" t="n">
-        <v>8571.5</v>
       </c>
       <c r="K38" t="n">
         <v>13228.625</v>
@@ -4826,31 +4826,31 @@
         <v>70</v>
       </c>
       <c r="B39" t="n">
+        <v>222.375</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
         <v>3408.25</v>
       </c>
-      <c r="C39" t="n">
+      <c r="F39" t="n">
         <v>3025.125</v>
       </c>
-      <c r="D39" t="n">
+      <c r="G39" t="n">
         <v>3097.5</v>
       </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
         <v>0.25</v>
-      </c>
-      <c r="H39" t="n">
-        <v>222.375</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" t="n">
-        <v>0</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -4933,31 +4933,31 @@
         <v>71</v>
       </c>
       <c r="B40" t="n">
+        <v>219.875</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E40" t="n">
         <v>109.75</v>
       </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
         <v>65.25</v>
       </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
-      </c>
       <c r="H40" t="n">
-        <v>219.875</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>3.25</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -5147,31 +5147,31 @@
         <v>73</v>
       </c>
       <c r="B42" t="n">
+        <v>7785.875</v>
+      </c>
+      <c r="C42" t="n">
+        <v>7567</v>
+      </c>
+      <c r="D42" t="n">
+        <v>7255</v>
+      </c>
+      <c r="E42" t="n">
         <v>7417</v>
       </c>
-      <c r="C42" t="n">
+      <c r="F42" t="n">
         <v>6996.375</v>
       </c>
-      <c r="D42" t="n">
+      <c r="G42" t="n">
         <v>7459.75</v>
       </c>
-      <c r="E42" t="n">
+      <c r="H42" t="n">
         <v>1275.375</v>
       </c>
-      <c r="F42" t="n">
+      <c r="I42" t="n">
         <v>603.625</v>
       </c>
-      <c r="G42" t="n">
+      <c r="J42" t="n">
         <v>1817.5</v>
-      </c>
-      <c r="H42" t="n">
-        <v>7785.875</v>
-      </c>
-      <c r="I42" t="n">
-        <v>7567</v>
-      </c>
-      <c r="J42" t="n">
-        <v>7255</v>
       </c>
       <c r="K42" t="n">
         <v>9428.375</v>
@@ -5254,31 +5254,31 @@
         <v>74</v>
       </c>
       <c r="B43" t="n">
+        <v>10479.625</v>
+      </c>
+      <c r="C43" t="n">
+        <v>9816.625</v>
+      </c>
+      <c r="D43" t="n">
+        <v>9465.25</v>
+      </c>
+      <c r="E43" t="n">
         <v>8474.75</v>
       </c>
-      <c r="C43" t="n">
+      <c r="F43" t="n">
         <v>8209.75</v>
       </c>
-      <c r="D43" t="n">
+      <c r="G43" t="n">
         <v>8029</v>
       </c>
-      <c r="E43" t="n">
+      <c r="H43" t="n">
         <v>90.375</v>
       </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" t="n">
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
         <v>200.875</v>
-      </c>
-      <c r="H43" t="n">
-        <v>10479.625</v>
-      </c>
-      <c r="I43" t="n">
-        <v>9816.625</v>
-      </c>
-      <c r="J43" t="n">
-        <v>9465.25</v>
       </c>
       <c r="K43" t="n">
         <v>6770</v>
@@ -5361,25 +5361,25 @@
         <v>75</v>
       </c>
       <c r="B44" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
         <v>3737.125</v>
       </c>
-      <c r="C44" t="n">
+      <c r="F44" t="n">
         <v>1682.625</v>
       </c>
-      <c r="D44" t="n">
+      <c r="G44" t="n">
         <v>3475.875</v>
       </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
       <c r="H44" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -5474,16 +5474,16 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
         <v>12.5</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -5575,16 +5575,16 @@
         <v>77</v>
       </c>
       <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
         <v>0.125</v>
-      </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -5697,16 +5697,16 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
         <v>0.25</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0</v>
-      </c>
-      <c r="J47" t="n">
-        <v>0</v>
       </c>
       <c r="K47" t="n">
         <v>0</v>
@@ -5789,31 +5789,31 @@
         <v>79</v>
       </c>
       <c r="B48" t="n">
+        <v>6717.875</v>
+      </c>
+      <c r="C48" t="n">
+        <v>5599.375</v>
+      </c>
+      <c r="D48" t="n">
+        <v>6180.375</v>
+      </c>
+      <c r="E48" t="n">
         <v>7570.875</v>
       </c>
-      <c r="C48" t="n">
+      <c r="F48" t="n">
         <v>7095</v>
       </c>
-      <c r="D48" t="n">
+      <c r="G48" t="n">
         <v>7251.5</v>
       </c>
-      <c r="E48" t="n">
+      <c r="H48" t="n">
         <v>2</v>
       </c>
-      <c r="F48" t="n">
+      <c r="I48" t="n">
         <v>17.25</v>
       </c>
-      <c r="G48" t="n">
+      <c r="J48" t="n">
         <v>2</v>
-      </c>
-      <c r="H48" t="n">
-        <v>6717.875</v>
-      </c>
-      <c r="I48" t="n">
-        <v>5599.375</v>
-      </c>
-      <c r="J48" t="n">
-        <v>6180.375</v>
       </c>
       <c r="K48" t="n">
         <v>1318.5</v>
@@ -5896,31 +5896,31 @@
         <v>80</v>
       </c>
       <c r="B49" t="n">
+        <v>54.75</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="D49" t="n">
+        <v>24</v>
+      </c>
+      <c r="E49" t="n">
         <v>653.875</v>
       </c>
-      <c r="C49" t="n">
+      <c r="F49" t="n">
         <v>49.625</v>
       </c>
-      <c r="D49" t="n">
+      <c r="G49" t="n">
         <v>634.125</v>
       </c>
-      <c r="E49" t="n">
+      <c r="H49" t="n">
         <v>465.75</v>
       </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
         <v>497.375</v>
-      </c>
-      <c r="H49" t="n">
-        <v>54.75</v>
-      </c>
-      <c r="I49" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="J49" t="n">
-        <v>24</v>
       </c>
       <c r="K49" t="n">
         <v>2.5</v>
@@ -6003,31 +6003,31 @@
         <v>81</v>
       </c>
       <c r="B50" t="n">
+        <v>11758.25</v>
+      </c>
+      <c r="C50" t="n">
+        <v>12104.625</v>
+      </c>
+      <c r="D50" t="n">
+        <v>11250.25</v>
+      </c>
+      <c r="E50" t="n">
         <v>13431.5</v>
       </c>
-      <c r="C50" t="n">
+      <c r="F50" t="n">
         <v>13610.75</v>
       </c>
-      <c r="D50" t="n">
+      <c r="G50" t="n">
         <v>12744</v>
       </c>
-      <c r="E50" t="n">
+      <c r="H50" t="n">
         <v>6704.125</v>
       </c>
-      <c r="F50" t="n">
+      <c r="I50" t="n">
         <v>6034.25</v>
       </c>
-      <c r="G50" t="n">
+      <c r="J50" t="n">
         <v>7347.5</v>
-      </c>
-      <c r="H50" t="n">
-        <v>11758.25</v>
-      </c>
-      <c r="I50" t="n">
-        <v>12104.625</v>
-      </c>
-      <c r="J50" t="n">
-        <v>11250.25</v>
       </c>
       <c r="K50" t="n">
         <v>13584.75</v>
@@ -6110,31 +6110,31 @@
         <v>82</v>
       </c>
       <c r="B51" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
         <v>1033.75</v>
       </c>
-      <c r="C51" t="n">
+      <c r="F51" t="n">
         <v>435.625</v>
       </c>
-      <c r="D51" t="n">
+      <c r="G51" t="n">
         <v>907.75</v>
       </c>
-      <c r="E51" t="n">
+      <c r="H51" t="n">
         <v>6</v>
       </c>
-      <c r="F51" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" t="n">
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
         <v>22.5</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>0</v>
       </c>
       <c r="K51" t="n">
         <v>6.25</v>
@@ -6330,25 +6330,25 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
         <v>5</v>
       </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
         <v>0.125</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="n">
-        <v>0</v>
       </c>
       <c r="K53" t="n">
         <v>0</v>
@@ -6431,31 +6431,31 @@
         <v>85</v>
       </c>
       <c r="B54" t="n">
+        <v>7727.75</v>
+      </c>
+      <c r="C54" t="n">
+        <v>6951.875</v>
+      </c>
+      <c r="D54" t="n">
+        <v>6863</v>
+      </c>
+      <c r="E54" t="n">
         <v>4379.375</v>
       </c>
-      <c r="C54" t="n">
+      <c r="F54" t="n">
         <v>3870.75</v>
       </c>
-      <c r="D54" t="n">
+      <c r="G54" t="n">
         <v>4981.625</v>
       </c>
-      <c r="E54" t="n">
+      <c r="H54" t="n">
         <v>2639.5</v>
       </c>
-      <c r="F54" t="n">
+      <c r="I54" t="n">
         <v>1824.25</v>
       </c>
-      <c r="G54" t="n">
+      <c r="J54" t="n">
         <v>2739</v>
-      </c>
-      <c r="H54" t="n">
-        <v>7727.75</v>
-      </c>
-      <c r="I54" t="n">
-        <v>6951.875</v>
-      </c>
-      <c r="J54" t="n">
-        <v>6863</v>
       </c>
       <c r="K54" t="n">
         <v>6469.625</v>
@@ -6538,22 +6538,22 @@
         <v>86</v>
       </c>
       <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
         <v>0.25</v>
       </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
         <v>10</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -6645,25 +6645,25 @@
         <v>87</v>
       </c>
       <c r="B56" t="n">
+        <v>6</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
         <v>109.625</v>
       </c>
-      <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="n">
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
         <v>262.75</v>
       </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
-      </c>
       <c r="H56" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -6752,31 +6752,31 @@
         <v>88</v>
       </c>
       <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
         <v>0.75</v>
       </c>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="n">
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
         <v>13.125</v>
       </c>
-      <c r="E57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
         <v>0.25</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0</v>
       </c>
       <c r="K57" t="n">
         <v>0</v>
@@ -6859,31 +6859,31 @@
         <v>89</v>
       </c>
       <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
         <v>3.5</v>
       </c>
-      <c r="C58" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" t="n">
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
         <v>4.25</v>
       </c>
-      <c r="E58" t="n">
+      <c r="H58" t="n">
         <v>0.25</v>
       </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
         <v>1.75</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0</v>
-      </c>
-      <c r="J58" t="n">
-        <v>0</v>
       </c>
       <c r="K58" t="n">
         <v>0</v>
@@ -6966,31 +6966,31 @@
         <v>90</v>
       </c>
       <c r="B59" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
         <v>73.75</v>
       </c>
-      <c r="C59" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" t="n">
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
         <v>160.875</v>
       </c>
-      <c r="E59" t="n">
+      <c r="H59" t="n">
         <v>3.75</v>
       </c>
-      <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
         <v>25.25</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" t="n">
-        <v>0</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -7073,7 +7073,7 @@
         <v>91</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
@@ -7088,16 +7088,16 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
         <v>0.25</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="I60" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" t="n">
-        <v>0</v>
       </c>
       <c r="K60" t="n">
         <v>0</v>
@@ -7180,31 +7180,31 @@
         <v>92</v>
       </c>
       <c r="B61" t="n">
+        <v>20.75</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E61" t="n">
         <v>24.375</v>
       </c>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="n">
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
         <v>71.125</v>
       </c>
-      <c r="E61" t="n">
+      <c r="H61" t="n">
         <v>283.25</v>
       </c>
-      <c r="F61" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="n">
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
         <v>241.5</v>
-      </c>
-      <c r="H61" t="n">
-        <v>20.75</v>
-      </c>
-      <c r="I61" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="J61" t="n">
-        <v>0.75</v>
       </c>
       <c r="K61" t="n">
         <v>1.75</v>
@@ -7287,31 +7287,31 @@
         <v>93</v>
       </c>
       <c r="B62" t="n">
+        <v>381.25</v>
+      </c>
+      <c r="C62" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="D62" t="n">
+        <v>223.625</v>
+      </c>
+      <c r="E62" t="n">
         <v>319.375</v>
       </c>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="n">
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
         <v>253.5</v>
       </c>
-      <c r="E62" t="n">
+      <c r="H62" t="n">
         <v>182.875</v>
       </c>
-      <c r="F62" t="n">
+      <c r="I62" t="n">
         <v>1</v>
       </c>
-      <c r="G62" t="n">
+      <c r="J62" t="n">
         <v>222.75</v>
-      </c>
-      <c r="H62" t="n">
-        <v>381.25</v>
-      </c>
-      <c r="I62" t="n">
-        <v>95.5</v>
-      </c>
-      <c r="J62" t="n">
-        <v>223.625</v>
       </c>
       <c r="K62" t="n">
         <v>12.75</v>
@@ -7394,31 +7394,31 @@
         <v>94</v>
       </c>
       <c r="B63" t="n">
+        <v>8099.5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>7898.75</v>
+      </c>
+      <c r="D63" t="n">
+        <v>7724.5</v>
+      </c>
+      <c r="E63" t="n">
         <v>7418.625</v>
       </c>
-      <c r="C63" t="n">
+      <c r="F63" t="n">
         <v>7983.375</v>
       </c>
-      <c r="D63" t="n">
+      <c r="G63" t="n">
         <v>8174.5</v>
       </c>
-      <c r="E63" t="n">
+      <c r="H63" t="n">
         <v>51.125</v>
       </c>
-      <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="n">
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
         <v>98.5</v>
-      </c>
-      <c r="H63" t="n">
-        <v>8099.5</v>
-      </c>
-      <c r="I63" t="n">
-        <v>7898.75</v>
-      </c>
-      <c r="J63" t="n">
-        <v>7724.5</v>
       </c>
       <c r="K63" t="n">
         <v>8917.75</v>
@@ -7501,31 +7501,31 @@
         <v>95</v>
       </c>
       <c r="B64" t="n">
+        <v>9864.875</v>
+      </c>
+      <c r="C64" t="n">
+        <v>9158.375</v>
+      </c>
+      <c r="D64" t="n">
+        <v>9049.25</v>
+      </c>
+      <c r="E64" t="n">
         <v>29.75</v>
       </c>
-      <c r="C64" t="n">
+      <c r="F64" t="n">
         <v>0.5</v>
       </c>
-      <c r="D64" t="n">
+      <c r="G64" t="n">
         <v>53.625</v>
       </c>
-      <c r="E64" t="n">
+      <c r="H64" t="n">
         <v>1</v>
       </c>
-      <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>0</v>
-      </c>
-      <c r="H64" t="n">
-        <v>9864.875</v>
-      </c>
       <c r="I64" t="n">
-        <v>9158.375</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>9049.25</v>
+        <v>0</v>
       </c>
       <c r="K64" t="n">
         <v>891.25</v>
@@ -7608,31 +7608,31 @@
         <v>96</v>
       </c>
       <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
         <v>347.75</v>
       </c>
-      <c r="C65" t="n">
+      <c r="F65" t="n">
         <v>0.5</v>
       </c>
-      <c r="D65" t="n">
+      <c r="G65" t="n">
         <v>402.625</v>
       </c>
-      <c r="E65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
         <v>1.5</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0</v>
-      </c>
-      <c r="I65" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" t="n">
-        <v>0</v>
       </c>
       <c r="K65" t="n">
         <v>0</v>
@@ -7715,31 +7715,31 @@
         <v>97</v>
       </c>
       <c r="B66" t="n">
+        <v>8545.625</v>
+      </c>
+      <c r="C66" t="n">
+        <v>7545.625</v>
+      </c>
+      <c r="D66" t="n">
+        <v>7615</v>
+      </c>
+      <c r="E66" t="n">
         <v>10430.5</v>
       </c>
-      <c r="C66" t="n">
+      <c r="F66" t="n">
         <v>9512.25</v>
       </c>
-      <c r="D66" t="n">
+      <c r="G66" t="n">
         <v>10572.5</v>
       </c>
-      <c r="E66" t="n">
+      <c r="H66" t="n">
         <v>4644.375</v>
       </c>
-      <c r="F66" t="n">
+      <c r="I66" t="n">
         <v>2911.875</v>
       </c>
-      <c r="G66" t="n">
+      <c r="J66" t="n">
         <v>5993.25</v>
-      </c>
-      <c r="H66" t="n">
-        <v>8545.625</v>
-      </c>
-      <c r="I66" t="n">
-        <v>7545.625</v>
-      </c>
-      <c r="J66" t="n">
-        <v>7615</v>
       </c>
       <c r="K66" t="n">
         <v>11415</v>
@@ -7822,31 +7822,31 @@
         <v>98</v>
       </c>
       <c r="B67" t="n">
+        <v>5356.25</v>
+      </c>
+      <c r="C67" t="n">
+        <v>4641.25</v>
+      </c>
+      <c r="D67" t="n">
+        <v>4493.5</v>
+      </c>
+      <c r="E67" t="n">
         <v>6878.75</v>
       </c>
-      <c r="C67" t="n">
+      <c r="F67" t="n">
         <v>5899.125</v>
       </c>
-      <c r="D67" t="n">
+      <c r="G67" t="n">
         <v>7087</v>
       </c>
-      <c r="E67" t="n">
+      <c r="H67" t="n">
         <v>2279.625</v>
       </c>
-      <c r="F67" t="n">
+      <c r="I67" t="n">
         <v>1335.25</v>
       </c>
-      <c r="G67" t="n">
+      <c r="J67" t="n">
         <v>2893.25</v>
-      </c>
-      <c r="H67" t="n">
-        <v>5356.25</v>
-      </c>
-      <c r="I67" t="n">
-        <v>4641.25</v>
-      </c>
-      <c r="J67" t="n">
-        <v>4493.5</v>
       </c>
       <c r="K67" t="n">
         <v>3274.5</v>
@@ -7929,31 +7929,31 @@
         <v>99</v>
       </c>
       <c r="B68" t="n">
+        <v>1983.625</v>
+      </c>
+      <c r="C68" t="n">
+        <v>902.75</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1401.75</v>
+      </c>
+      <c r="E68" t="n">
         <v>3031.625</v>
       </c>
-      <c r="C68" t="n">
+      <c r="F68" t="n">
         <v>1983.625</v>
       </c>
-      <c r="D68" t="n">
+      <c r="G68" t="n">
         <v>3643.5</v>
       </c>
-      <c r="E68" t="n">
-        <v>0</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="n">
-        <v>0</v>
-      </c>
       <c r="H68" t="n">
-        <v>1983.625</v>
+        <v>0</v>
       </c>
       <c r="I68" t="n">
-        <v>902.75</v>
+        <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>1401.75</v>
+        <v>0</v>
       </c>
       <c r="K68" t="n">
         <v>886.25</v>
@@ -8036,31 +8036,31 @@
         <v>100</v>
       </c>
       <c r="B69" t="n">
+        <v>9509.125</v>
+      </c>
+      <c r="C69" t="n">
+        <v>9010.5</v>
+      </c>
+      <c r="D69" t="n">
+        <v>8764.25</v>
+      </c>
+      <c r="E69" t="n">
         <v>9366</v>
       </c>
-      <c r="C69" t="n">
+      <c r="F69" t="n">
         <v>8366.625</v>
       </c>
-      <c r="D69" t="n">
+      <c r="G69" t="n">
         <v>8095.5</v>
       </c>
-      <c r="E69" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
-        <v>0</v>
-      </c>
       <c r="H69" t="n">
-        <v>9509.125</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
-        <v>9010.5</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>8764.25</v>
+        <v>0</v>
       </c>
       <c r="K69" t="n">
         <v>645</v>
@@ -8149,25 +8149,25 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
         <v>3.5</v>
       </c>
-      <c r="E70" t="n">
+      <c r="H70" t="n">
         <v>1</v>
       </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
         <v>2.75</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J70" t="n">
-        <v>0</v>
       </c>
       <c r="K70" t="n">
         <v>2833.625</v>
@@ -8250,31 +8250,31 @@
         <v>102</v>
       </c>
       <c r="B71" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>20.25</v>
+      </c>
+      <c r="E71" t="n">
         <v>413.625</v>
       </c>
-      <c r="C71" t="n">
+      <c r="F71" t="n">
         <v>2.375</v>
       </c>
-      <c r="D71" t="n">
+      <c r="G71" t="n">
         <v>337.25</v>
       </c>
-      <c r="E71" t="n">
+      <c r="H71" t="n">
         <v>15.75</v>
       </c>
-      <c r="F71" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" t="n">
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
         <v>46</v>
-      </c>
-      <c r="H71" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="I71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J71" t="n">
-        <v>20.25</v>
       </c>
       <c r="K71" t="n">
         <v>3.25</v>
@@ -8357,31 +8357,31 @@
         <v>103</v>
       </c>
       <c r="B72" t="n">
+        <v>146.25</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D72" t="n">
+        <v>10</v>
+      </c>
+      <c r="E72" t="n">
         <v>831.75</v>
       </c>
-      <c r="C72" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" t="n">
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
         <v>453.875</v>
       </c>
-      <c r="E72" t="n">
+      <c r="H72" t="n">
         <v>179.25</v>
       </c>
-      <c r="F72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" t="n">
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
         <v>213.5</v>
-      </c>
-      <c r="H72" t="n">
-        <v>146.25</v>
-      </c>
-      <c r="I72" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="J72" t="n">
-        <v>10</v>
       </c>
       <c r="K72" t="n">
         <v>2</v>
@@ -8464,31 +8464,31 @@
         <v>104</v>
       </c>
       <c r="B73" t="n">
+        <v>324.125</v>
+      </c>
+      <c r="C73" t="n">
+        <v>72.25</v>
+      </c>
+      <c r="D73" t="n">
+        <v>171</v>
+      </c>
+      <c r="E73" t="n">
         <v>655.375</v>
       </c>
-      <c r="C73" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" t="n">
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
         <v>647.125</v>
       </c>
-      <c r="E73" t="n">
+      <c r="H73" t="n">
         <v>388</v>
       </c>
-      <c r="F73" t="n">
+      <c r="I73" t="n">
         <v>0.25</v>
       </c>
-      <c r="G73" t="n">
+      <c r="J73" t="n">
         <v>396.75</v>
-      </c>
-      <c r="H73" t="n">
-        <v>324.125</v>
-      </c>
-      <c r="I73" t="n">
-        <v>72.25</v>
-      </c>
-      <c r="J73" t="n">
-        <v>171</v>
       </c>
       <c r="K73" t="n">
         <v>98.625</v>
@@ -8571,31 +8571,31 @@
         <v>105</v>
       </c>
       <c r="B74" t="n">
+        <v>627.875</v>
+      </c>
+      <c r="C74" t="n">
+        <v>15.75</v>
+      </c>
+      <c r="D74" t="n">
+        <v>117.5</v>
+      </c>
+      <c r="E74" t="n">
         <v>292.25</v>
       </c>
-      <c r="C74" t="n">
-        <v>0</v>
-      </c>
-      <c r="D74" t="n">
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
         <v>336.75</v>
       </c>
-      <c r="E74" t="n">
+      <c r="H74" t="n">
         <v>285</v>
       </c>
-      <c r="F74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="n">
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
         <v>263.625</v>
-      </c>
-      <c r="H74" t="n">
-        <v>627.875</v>
-      </c>
-      <c r="I74" t="n">
-        <v>15.75</v>
-      </c>
-      <c r="J74" t="n">
-        <v>117.5</v>
       </c>
       <c r="K74" t="n">
         <v>147.25</v>
@@ -8678,31 +8678,31 @@
         <v>106</v>
       </c>
       <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
         <v>0.5</v>
       </c>
-      <c r="C75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D75" t="n">
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
         <v>9.75</v>
       </c>
-      <c r="E75" t="n">
+      <c r="H75" t="n">
         <v>19</v>
       </c>
-      <c r="F75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="n">
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
         <v>34.5</v>
-      </c>
-      <c r="H75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J75" t="n">
-        <v>0</v>
       </c>
       <c r="K75" t="n">
         <v>0</v>
@@ -8785,31 +8785,31 @@
         <v>107</v>
       </c>
       <c r="B76" t="n">
+        <v>3389.875</v>
+      </c>
+      <c r="C76" t="n">
+        <v>3301.375</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1928.875</v>
+      </c>
+      <c r="E76" t="n">
         <v>6034.375</v>
       </c>
-      <c r="C76" t="n">
+      <c r="F76" t="n">
         <v>5519</v>
       </c>
-      <c r="D76" t="n">
+      <c r="G76" t="n">
         <v>6232.5</v>
       </c>
-      <c r="E76" t="n">
+      <c r="H76" t="n">
         <v>82.5</v>
       </c>
-      <c r="F76" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" t="n">
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
         <v>278.25</v>
-      </c>
-      <c r="H76" t="n">
-        <v>3389.875</v>
-      </c>
-      <c r="I76" t="n">
-        <v>3301.375</v>
-      </c>
-      <c r="J76" t="n">
-        <v>1928.875</v>
       </c>
       <c r="K76" t="n">
         <v>1694.25</v>
@@ -8892,31 +8892,31 @@
         <v>108</v>
       </c>
       <c r="B77" t="n">
+        <v>4319.125</v>
+      </c>
+      <c r="C77" t="n">
+        <v>3454.5</v>
+      </c>
+      <c r="D77" t="n">
+        <v>3376.125</v>
+      </c>
+      <c r="E77" t="n">
         <v>7208</v>
       </c>
-      <c r="C77" t="n">
+      <c r="F77" t="n">
         <v>6967.25</v>
       </c>
-      <c r="D77" t="n">
+      <c r="G77" t="n">
         <v>7236.625</v>
       </c>
-      <c r="E77" t="n">
+      <c r="H77" t="n">
         <v>1.75</v>
       </c>
-      <c r="F77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" t="n">
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
         <v>5</v>
-      </c>
-      <c r="H77" t="n">
-        <v>4319.125</v>
-      </c>
-      <c r="I77" t="n">
-        <v>3454.5</v>
-      </c>
-      <c r="J77" t="n">
-        <v>3376.125</v>
       </c>
       <c r="K77" t="n">
         <v>364.5</v>
@@ -8999,31 +8999,31 @@
         <v>109</v>
       </c>
       <c r="B78" t="n">
+        <v>5053</v>
+      </c>
+      <c r="C78" t="n">
+        <v>4487.25</v>
+      </c>
+      <c r="D78" t="n">
+        <v>4687.375</v>
+      </c>
+      <c r="E78" t="n">
         <v>10000.5</v>
       </c>
-      <c r="C78" t="n">
+      <c r="F78" t="n">
         <v>9690.25</v>
       </c>
-      <c r="D78" t="n">
+      <c r="G78" t="n">
         <v>10291.875</v>
       </c>
-      <c r="E78" t="n">
+      <c r="H78" t="n">
         <v>2722</v>
       </c>
-      <c r="F78" t="n">
+      <c r="I78" t="n">
         <v>1420.625</v>
       </c>
-      <c r="G78" t="n">
+      <c r="J78" t="n">
         <v>3080.125</v>
-      </c>
-      <c r="H78" t="n">
-        <v>5053</v>
-      </c>
-      <c r="I78" t="n">
-        <v>4487.25</v>
-      </c>
-      <c r="J78" t="n">
-        <v>4687.375</v>
       </c>
       <c r="K78" t="n">
         <v>7675.5</v>
@@ -9106,31 +9106,31 @@
         <v>110</v>
       </c>
       <c r="B79" t="n">
+        <v>145.25</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" t="n">
+        <v>33.25</v>
+      </c>
+      <c r="E79" t="n">
         <v>74.375</v>
       </c>
-      <c r="C79" t="n">
-        <v>0</v>
-      </c>
-      <c r="D79" t="n">
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
         <v>35.75</v>
       </c>
-      <c r="E79" t="n">
+      <c r="H79" t="n">
         <v>21.25</v>
       </c>
-      <c r="F79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" t="n">
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="n">
         <v>56.5</v>
-      </c>
-      <c r="H79" t="n">
-        <v>145.25</v>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="n">
-        <v>33.25</v>
       </c>
       <c r="K79" t="n">
         <v>0</v>
@@ -9213,31 +9213,31 @@
         <v>111</v>
       </c>
       <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
         <v>1</v>
       </c>
-      <c r="C80" t="n">
-        <v>0</v>
-      </c>
-      <c r="D80" t="n">
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
         <v>2.25</v>
       </c>
-      <c r="E80" t="n">
+      <c r="H80" t="n">
         <v>1.25</v>
       </c>
-      <c r="F80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" t="n">
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
         <v>7.5</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0</v>
-      </c>
-      <c r="I80" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0</v>
       </c>
       <c r="K80" t="n">
         <v>0.25</v>
@@ -9320,31 +9320,31 @@
         <v>112</v>
       </c>
       <c r="B81" t="n">
+        <v>6</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
         <v>11.25</v>
       </c>
-      <c r="C81" t="n">
-        <v>0</v>
-      </c>
-      <c r="D81" t="n">
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
         <v>47.625</v>
       </c>
-      <c r="E81" t="n">
+      <c r="H81" t="n">
         <v>0.5</v>
       </c>
-      <c r="F81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" t="n">
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
         <v>4.25</v>
-      </c>
-      <c r="H81" t="n">
-        <v>6</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0</v>
-      </c>
-      <c r="J81" t="n">
-        <v>0</v>
       </c>
       <c r="K81" t="n">
         <v>0</v>
@@ -9427,31 +9427,31 @@
         <v>113</v>
       </c>
       <c r="B82" t="n">
+        <v>6693.625</v>
+      </c>
+      <c r="C82" t="n">
+        <v>5169.75</v>
+      </c>
+      <c r="D82" t="n">
+        <v>5537.125</v>
+      </c>
+      <c r="E82" t="n">
         <v>586.875</v>
       </c>
-      <c r="C82" t="n">
-        <v>0</v>
-      </c>
-      <c r="D82" t="n">
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
         <v>287</v>
       </c>
-      <c r="E82" t="n">
+      <c r="H82" t="n">
         <v>853.75</v>
       </c>
-      <c r="F82" t="n">
+      <c r="I82" t="n">
         <v>49.375</v>
       </c>
-      <c r="G82" t="n">
+      <c r="J82" t="n">
         <v>2099.5</v>
-      </c>
-      <c r="H82" t="n">
-        <v>6693.625</v>
-      </c>
-      <c r="I82" t="n">
-        <v>5169.75</v>
-      </c>
-      <c r="J82" t="n">
-        <v>5537.125</v>
       </c>
       <c r="K82" t="n">
         <v>10714.875</v>
@@ -9534,31 +9534,31 @@
         <v>114</v>
       </c>
       <c r="B83" t="n">
+        <v>9485.25</v>
+      </c>
+      <c r="C83" t="n">
+        <v>8908.625</v>
+      </c>
+      <c r="D83" t="n">
+        <v>8598.125</v>
+      </c>
+      <c r="E83" t="n">
         <v>9875.75</v>
       </c>
-      <c r="C83" t="n">
+      <c r="F83" t="n">
         <v>7204.75</v>
       </c>
-      <c r="D83" t="n">
+      <c r="G83" t="n">
         <v>9322.75</v>
       </c>
-      <c r="E83" t="n">
+      <c r="H83" t="n">
         <v>5035.375</v>
       </c>
-      <c r="F83" t="n">
+      <c r="I83" t="n">
         <v>3439.25</v>
       </c>
-      <c r="G83" t="n">
+      <c r="J83" t="n">
         <v>6599.5</v>
-      </c>
-      <c r="H83" t="n">
-        <v>9485.25</v>
-      </c>
-      <c r="I83" t="n">
-        <v>8908.625</v>
-      </c>
-      <c r="J83" t="n">
-        <v>8598.125</v>
       </c>
       <c r="K83" t="n">
         <v>7870.75</v>
@@ -9641,31 +9641,31 @@
         <v>115</v>
       </c>
       <c r="B84" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>12</v>
+      </c>
+      <c r="E84" t="n">
         <v>968.375</v>
       </c>
-      <c r="C84" t="n">
-        <v>0</v>
-      </c>
-      <c r="D84" t="n">
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
         <v>920.5</v>
       </c>
-      <c r="E84" t="n">
+      <c r="H84" t="n">
         <v>630.5</v>
       </c>
-      <c r="F84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="n">
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
         <v>581.5</v>
-      </c>
-      <c r="H84" t="n">
-        <v>82.5</v>
-      </c>
-      <c r="I84" t="n">
-        <v>0</v>
-      </c>
-      <c r="J84" t="n">
-        <v>12</v>
       </c>
       <c r="K84" t="n">
         <v>2</v>
@@ -9748,31 +9748,31 @@
         <v>116</v>
       </c>
       <c r="B85" t="n">
+        <v>9858.375</v>
+      </c>
+      <c r="C85" t="n">
+        <v>9046.25</v>
+      </c>
+      <c r="D85" t="n">
+        <v>8504</v>
+      </c>
+      <c r="E85" t="n">
         <v>11952.25</v>
       </c>
-      <c r="C85" t="n">
+      <c r="F85" t="n">
         <v>11936.75</v>
       </c>
-      <c r="D85" t="n">
+      <c r="G85" t="n">
         <v>12213.5</v>
       </c>
-      <c r="E85" t="n">
+      <c r="H85" t="n">
         <v>2088.625</v>
       </c>
-      <c r="F85" t="n">
+      <c r="I85" t="n">
         <v>4452.125</v>
       </c>
-      <c r="G85" t="n">
+      <c r="J85" t="n">
         <v>3778</v>
-      </c>
-      <c r="H85" t="n">
-        <v>9858.375</v>
-      </c>
-      <c r="I85" t="n">
-        <v>9046.25</v>
-      </c>
-      <c r="J85" t="n">
-        <v>8504</v>
       </c>
       <c r="K85" t="n">
         <v>12885.875</v>
@@ -9855,31 +9855,31 @@
         <v>117</v>
       </c>
       <c r="B86" t="n">
+        <v>897.875</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D86" t="n">
+        <v>222.625</v>
+      </c>
+      <c r="E86" t="n">
         <v>1081.5</v>
       </c>
-      <c r="C86" t="n">
-        <v>0</v>
-      </c>
-      <c r="D86" t="n">
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
         <v>1105.5</v>
       </c>
-      <c r="E86" t="n">
+      <c r="H86" t="n">
         <v>972.125</v>
       </c>
-      <c r="F86" t="n">
-        <v>0</v>
-      </c>
-      <c r="G86" t="n">
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
         <v>1009</v>
-      </c>
-      <c r="H86" t="n">
-        <v>897.875</v>
-      </c>
-      <c r="I86" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J86" t="n">
-        <v>222.625</v>
       </c>
       <c r="K86" t="n">
         <v>426.625</v>
@@ -9962,31 +9962,31 @@
         <v>118</v>
       </c>
       <c r="B87" t="n">
+        <v>2208.25</v>
+      </c>
+      <c r="C87" t="n">
+        <v>483.25</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1407.25</v>
+      </c>
+      <c r="E87" t="n">
         <v>1072.75</v>
       </c>
-      <c r="C87" t="n">
+      <c r="F87" t="n">
         <v>156.5</v>
       </c>
-      <c r="D87" t="n">
+      <c r="G87" t="n">
         <v>1118.125</v>
       </c>
-      <c r="E87" t="n">
+      <c r="H87" t="n">
         <v>188.5</v>
       </c>
-      <c r="F87" t="n">
-        <v>0</v>
-      </c>
-      <c r="G87" t="n">
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="n">
         <v>196.625</v>
-      </c>
-      <c r="H87" t="n">
-        <v>2208.25</v>
-      </c>
-      <c r="I87" t="n">
-        <v>483.25</v>
-      </c>
-      <c r="J87" t="n">
-        <v>1407.25</v>
       </c>
       <c r="K87" t="n">
         <v>956.25</v>
@@ -10069,31 +10069,31 @@
         <v>119</v>
       </c>
       <c r="B88" t="n">
+        <v>69</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E88" t="n">
         <v>106.625</v>
       </c>
-      <c r="C88" t="n">
-        <v>0</v>
-      </c>
-      <c r="D88" t="n">
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
         <v>83.375</v>
       </c>
-      <c r="E88" t="n">
+      <c r="H88" t="n">
         <v>77.875</v>
       </c>
-      <c r="F88" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" t="n">
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
         <v>118.75</v>
-      </c>
-      <c r="H88" t="n">
-        <v>69</v>
-      </c>
-      <c r="I88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J88" t="n">
-        <v>0.25</v>
       </c>
       <c r="K88" t="n">
         <v>7.75</v>
@@ -10176,31 +10176,31 @@
         <v>120</v>
       </c>
       <c r="B89" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
         <v>6</v>
       </c>
-      <c r="C89" t="n">
-        <v>0</v>
-      </c>
-      <c r="D89" t="n">
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
         <v>7</v>
       </c>
-      <c r="E89" t="n">
+      <c r="H89" t="n">
         <v>28.75</v>
       </c>
-      <c r="F89" t="n">
-        <v>0</v>
-      </c>
-      <c r="G89" t="n">
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="n">
         <v>48.125</v>
-      </c>
-      <c r="H89" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="I89" t="n">
-        <v>0</v>
-      </c>
-      <c r="J89" t="n">
-        <v>0</v>
       </c>
       <c r="K89" t="n">
         <v>0.25</v>
@@ -10283,31 +10283,31 @@
         <v>121</v>
       </c>
       <c r="B90" t="n">
+        <v>108.875</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="E90" t="n">
         <v>635.875</v>
       </c>
-      <c r="C90" t="n">
-        <v>0</v>
-      </c>
-      <c r="D90" t="n">
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
         <v>545.75</v>
       </c>
-      <c r="E90" t="n">
+      <c r="H90" t="n">
         <v>122.625</v>
       </c>
-      <c r="F90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="n">
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
         <v>212.625</v>
-      </c>
-      <c r="H90" t="n">
-        <v>108.875</v>
-      </c>
-      <c r="I90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J90" t="n">
-        <v>2.25</v>
       </c>
       <c r="K90" t="n">
         <v>45.375</v>
@@ -10390,31 +10390,31 @@
         <v>122</v>
       </c>
       <c r="B91" t="n">
+        <v>1266.875</v>
+      </c>
+      <c r="C91" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="D91" t="n">
+        <v>427.875</v>
+      </c>
+      <c r="E91" t="n">
         <v>895.75</v>
       </c>
-      <c r="C91" t="n">
-        <v>0</v>
-      </c>
-      <c r="D91" t="n">
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
         <v>973</v>
       </c>
-      <c r="E91" t="n">
+      <c r="H91" t="n">
         <v>830</v>
       </c>
-      <c r="F91" t="n">
+      <c r="I91" t="n">
         <v>1</v>
       </c>
-      <c r="G91" t="n">
+      <c r="J91" t="n">
         <v>930.25</v>
-      </c>
-      <c r="H91" t="n">
-        <v>1266.875</v>
-      </c>
-      <c r="I91" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="J91" t="n">
-        <v>427.875</v>
       </c>
       <c r="K91" t="n">
         <v>473.75</v>
@@ -10497,31 +10497,31 @@
         <v>123</v>
       </c>
       <c r="B92" t="n">
+        <v>608.625</v>
+      </c>
+      <c r="C92" t="n">
+        <v>37.25</v>
+      </c>
+      <c r="D92" t="n">
+        <v>448</v>
+      </c>
+      <c r="E92" t="n">
         <v>1122.125</v>
       </c>
-      <c r="C92" t="n">
-        <v>0</v>
-      </c>
-      <c r="D92" t="n">
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
         <v>1002.75</v>
       </c>
-      <c r="E92" t="n">
+      <c r="H92" t="n">
         <v>624.125</v>
       </c>
-      <c r="F92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" t="n">
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
         <v>622.875</v>
-      </c>
-      <c r="H92" t="n">
-        <v>608.625</v>
-      </c>
-      <c r="I92" t="n">
-        <v>37.25</v>
-      </c>
-      <c r="J92" t="n">
-        <v>448</v>
       </c>
       <c r="K92" t="n">
         <v>522.25</v>
@@ -10604,31 +10604,31 @@
         <v>124</v>
       </c>
       <c r="B93" t="n">
+        <v>10123.5</v>
+      </c>
+      <c r="C93" t="n">
+        <v>9106</v>
+      </c>
+      <c r="D93" t="n">
+        <v>8470.375</v>
+      </c>
+      <c r="E93" t="n">
         <v>10885.25</v>
       </c>
-      <c r="C93" t="n">
+      <c r="F93" t="n">
         <v>9276.875</v>
       </c>
-      <c r="D93" t="n">
+      <c r="G93" t="n">
         <v>11190.75</v>
       </c>
-      <c r="E93" t="n">
+      <c r="H93" t="n">
         <v>4623.125</v>
       </c>
-      <c r="F93" t="n">
+      <c r="I93" t="n">
         <v>3051.375</v>
       </c>
-      <c r="G93" t="n">
+      <c r="J93" t="n">
         <v>6857.25</v>
-      </c>
-      <c r="H93" t="n">
-        <v>10123.5</v>
-      </c>
-      <c r="I93" t="n">
-        <v>9106</v>
-      </c>
-      <c r="J93" t="n">
-        <v>8470.375</v>
       </c>
       <c r="K93" t="n">
         <v>8716.875</v>
@@ -10711,31 +10711,31 @@
         <v>125</v>
       </c>
       <c r="B94" t="n">
+        <v>123</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E94" t="n">
         <v>2131.625</v>
       </c>
-      <c r="C94" t="n">
+      <c r="F94" t="n">
         <v>813.625</v>
       </c>
-      <c r="D94" t="n">
+      <c r="G94" t="n">
         <v>2174.75</v>
       </c>
-      <c r="E94" t="n">
+      <c r="H94" t="n">
         <v>676</v>
       </c>
-      <c r="F94" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="n">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="n">
         <v>660.875</v>
-      </c>
-      <c r="H94" t="n">
-        <v>123</v>
-      </c>
-      <c r="I94" t="n">
-        <v>0</v>
-      </c>
-      <c r="J94" t="n">
-        <v>1.25</v>
       </c>
       <c r="K94" t="n">
         <v>37.5</v>
@@ -10818,31 +10818,31 @@
         <v>126</v>
       </c>
       <c r="B95" t="n">
+        <v>7692.25</v>
+      </c>
+      <c r="C95" t="n">
+        <v>6785.25</v>
+      </c>
+      <c r="D95" t="n">
+        <v>6676.625</v>
+      </c>
+      <c r="E95" t="n">
         <v>6080.875</v>
       </c>
-      <c r="C95" t="n">
+      <c r="F95" t="n">
         <v>6007.25</v>
       </c>
-      <c r="D95" t="n">
+      <c r="G95" t="n">
         <v>5870.125</v>
       </c>
-      <c r="E95" t="n">
+      <c r="H95" t="n">
         <v>814.75</v>
       </c>
-      <c r="F95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" t="n">
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="n">
         <v>832.625</v>
-      </c>
-      <c r="H95" t="n">
-        <v>7692.25</v>
-      </c>
-      <c r="I95" t="n">
-        <v>6785.25</v>
-      </c>
-      <c r="J95" t="n">
-        <v>6676.625</v>
       </c>
       <c r="K95" t="n">
         <v>9960.75</v>
@@ -10925,31 +10925,31 @@
         <v>127</v>
       </c>
       <c r="B96" t="n">
+        <v>90.25</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="E96" t="n">
         <v>906.625</v>
       </c>
-      <c r="C96" t="n">
-        <v>0</v>
-      </c>
-      <c r="D96" t="n">
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
         <v>978</v>
       </c>
-      <c r="E96" t="n">
+      <c r="H96" t="n">
         <v>968.5</v>
       </c>
-      <c r="F96" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="n">
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" t="n">
         <v>878</v>
-      </c>
-      <c r="H96" t="n">
-        <v>90.25</v>
-      </c>
-      <c r="I96" t="n">
-        <v>0</v>
-      </c>
-      <c r="J96" t="n">
-        <v>5.75</v>
       </c>
       <c r="K96" t="n">
         <v>11.25</v>
@@ -11032,31 +11032,31 @@
         <v>128</v>
       </c>
       <c r="B97" t="n">
+        <v>1173.5</v>
+      </c>
+      <c r="C97" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="D97" t="n">
+        <v>808.75</v>
+      </c>
+      <c r="E97" t="n">
         <v>1091.5</v>
       </c>
-      <c r="C97" t="n">
+      <c r="F97" t="n">
         <v>4.75</v>
       </c>
-      <c r="D97" t="n">
+      <c r="G97" t="n">
         <v>1117.375</v>
       </c>
-      <c r="E97" t="n">
+      <c r="H97" t="n">
         <v>1087.375</v>
       </c>
-      <c r="F97" t="n">
+      <c r="I97" t="n">
         <v>1</v>
       </c>
-      <c r="G97" t="n">
+      <c r="J97" t="n">
         <v>1024</v>
-      </c>
-      <c r="H97" t="n">
-        <v>1173.5</v>
-      </c>
-      <c r="I97" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="J97" t="n">
-        <v>808.75</v>
       </c>
       <c r="K97" t="n">
         <v>597.625</v>

</xml_diff>